<commit_message>
Fixed the incidence and prevalance code. Created table 8-9. Worked on the methods section and re-written the results table.
</commit_message>
<xml_diff>
--- a/Results/Asthma_IR.xlsx
+++ b/Results/Asthma_IR.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="57">
   <si>
     <t>FIPS</t>
   </si>
@@ -273,15 +273,9 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>285.2842079686713</v>
-      </c>
-      <c r="D3" t="n">
-        <v>170269.95115216108</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.6754818218848737</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -415,15 +409,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="n">
-        <v>3536.9048151857473</v>
-      </c>
-      <c r="D13" t="n">
-        <v>242105.48897986798</v>
-      </c>
-      <c r="E13" t="n">
-        <v>14.608941045032873</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -941,24 +929,6 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1008,15 +978,9 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
-        <v>1177.0366267393229</v>
-      </c>
-      <c r="D3" t="n">
-        <v>168778.7001084394</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6.973845787312517</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1154,15 +1118,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="n">
-        <v>2728.042383331478</v>
-      </c>
-      <c r="D13" t="n">
-        <v>252405.23293800003</v>
-      </c>
-      <c r="E13" t="n">
-        <v>10.80818472571678</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1724,33 +1682,6 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1922,15 +1853,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="n">
-        <v>4428.106627941318</v>
-      </c>
-      <c r="D13" t="n">
-        <v>241074.57606812636</v>
-      </c>
-      <c r="E13" t="n">
-        <v>18.368202488054813</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2470,33 +2395,6 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -2668,15 +2566,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="n">
-        <v>4339.823157976298</v>
-      </c>
-      <c r="D13" t="n">
-        <v>236873.12041212153</v>
-      </c>
-      <c r="E13" t="n">
-        <v>18.321298551839465</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -3202,39 +3094,6 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54" t="n">
-        <v>12429.083969815472</v>
-      </c>
-      <c r="D54" t="n">
-        <v>801519.2864594345</v>
-      </c>
-      <c r="E54" t="n">
-        <v>15.506905672499395</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3406,15 +3265,9 @@
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="n">
-        <v>5137.321733904018</v>
-      </c>
-      <c r="D13" t="n">
-        <v>241186.5409312679</v>
-      </c>
-      <c r="E13" t="n">
-        <v>21.300200724583657</v>
-      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -3934,33 +3787,6 @@
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>66.0</v>
-      </c>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -3994,579 +3820,545 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>1747.6050426766656</v>
+        <v>42621.918836024626</v>
       </c>
       <c r="D2" t="n">
-        <v>509318.60241276154</v>
+        <v>2802421.7470672023</v>
       </c>
       <c r="E2" t="n">
-        <v>3.4312609718118505</v>
+        <v>15.208959493919652</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>75677.80092400518</v>
+        <v>156599.0264181489</v>
       </c>
       <c r="D3" t="n">
-        <v>4195573.812142029</v>
+        <v>1.6850453394726697E7</v>
       </c>
       <c r="E3" t="n">
-        <v>18.03753296032903</v>
+        <v>9.29346070101331</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6.0</v>
+        <v>9.0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>257764.54264810268</v>
+        <v>32938.5229378051</v>
       </c>
       <c r="D4" t="n">
-        <v>2.5213269728264272E7</v>
+        <v>2734477.7688722718</v>
       </c>
       <c r="E4" t="n">
-        <v>10.223368306695527</v>
+        <v>12.045635664973537</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>32938.5229378051</v>
+        <v>3184.446344618885</v>
       </c>
       <c r="D5" t="n">
-        <v>2734477.7688722718</v>
+        <v>179492.85599165817</v>
       </c>
       <c r="E5" t="n">
-        <v>12.045635664973537</v>
+        <v>17.74135425627681</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>3632.4067158099247</v>
+        <v>94786.03809289802</v>
       </c>
       <c r="D6" t="n">
-        <v>263899.71828849113</v>
+        <v>1.0458073543508092E7</v>
       </c>
       <c r="E6" t="n">
-        <v>13.764344802517119</v>
+        <v>9.063431969431596</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>107611.47674052886</v>
+        <v>37799.24289699028</v>
       </c>
       <c r="D7" t="n">
-        <v>1.2461910448594186E7</v>
+        <v>5673571.265652148</v>
       </c>
       <c r="E7" t="n">
-        <v>8.635231105570044</v>
+        <v>6.662336846956915</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="n">
-        <v>23707.103533524605</v>
+        <v>105218.93189138013</v>
       </c>
       <c r="D8" t="n">
-        <v>1455750.4483092518</v>
+        <v>6936762.371679282</v>
       </c>
       <c r="E8" t="n">
-        <v>16.285142526357234</v>
+        <v>15.168305652354107</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="n">
-        <v>37799.24289699028</v>
+        <v>11510.486502884885</v>
       </c>
       <c r="D9" t="n">
-        <v>5673571.265652148</v>
+        <v>1829733.9661702944</v>
       </c>
       <c r="E9" t="n">
-        <v>6.662336846956915</v>
+        <v>6.290797851327419</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>18.0</v>
+        <v>20.0</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>141200.38749005896</v>
+        <v>27509.487892604753</v>
       </c>
       <c r="D10" t="n">
-        <v>8351486.190213702</v>
+        <v>3059760.3617240055</v>
       </c>
       <c r="E10" t="n">
-        <v>16.907216784423117</v>
+        <v>8.990732815789757</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>19.0</v>
+        <v>22.0</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C11" t="n">
-        <v>14589.418409442658</v>
+        <v>5378.786540781787</v>
       </c>
       <c r="D11" t="n">
-        <v>2449462.8921591653</v>
+        <v>931966.3594570106</v>
       </c>
       <c r="E11" t="n">
-        <v>5.956170414397379</v>
+        <v>5.771438514063552</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>20.0</v>
+        <v>23.0</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C12" t="n">
-        <v>32245.24959672446</v>
+        <v>6662.149701015229</v>
       </c>
       <c r="D12" t="n">
-        <v>3663274.8746109568</v>
+        <v>722763.1937653258</v>
       </c>
       <c r="E12" t="n">
-        <v>8.802301410742194</v>
+        <v>9.217610634415294</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C13" t="n">
-        <v>5378.786540781787</v>
+        <v>64870.5736086545</v>
       </c>
       <c r="D13" t="n">
-        <v>931966.3594570106</v>
+        <v>5816583.904105316</v>
       </c>
       <c r="E13" t="n">
-        <v>5.771438514063552</v>
+        <v>11.152692831073782</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>23.0</v>
+        <v>26.0</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" t="n">
-        <v>9863.394304900807</v>
+        <v>126101.97053771566</v>
       </c>
       <c r="D14" t="n">
-        <v>969001.0600684974</v>
+        <v>1.0491065363787048E7</v>
       </c>
       <c r="E14" t="n">
-        <v>10.178930355559752</v>
+        <v>12.0199394594369</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C15" t="n">
-        <v>84556.5271466981</v>
+        <v>18264.008952066375</v>
       </c>
       <c r="D15" t="n">
-        <v>7030420.441808348</v>
+        <v>1300916.7417331804</v>
       </c>
       <c r="E15" t="n">
-        <v>12.027236186879982</v>
+        <v>14.039337312035567</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>26.0</v>
+        <v>29.0</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" t="n">
-        <v>137666.80576710775</v>
+        <v>46410.034572168624</v>
       </c>
       <c r="D16" t="n">
-        <v>1.2676714593852432E7</v>
+        <v>3600272.063188931</v>
       </c>
       <c r="E16" t="n">
-        <v>10.859817403625165</v>
+        <v>12.890702079625912</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="n">
-        <v>18264.008952066375</v>
+        <v>3295.889765187216</v>
       </c>
       <c r="D17" t="n">
-        <v>1300916.7417331804</v>
+        <v>768012.0066596719</v>
       </c>
       <c r="E17" t="n">
-        <v>14.039337312035567</v>
+        <v>4.291456040540417</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>29.0</v>
+        <v>31.0</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" t="n">
-        <v>71848.34476078108</v>
+        <v>18262.226573581298</v>
       </c>
       <c r="D18" t="n">
-        <v>4801190.887420368</v>
+        <v>2014605.1364890952</v>
       </c>
       <c r="E18" t="n">
-        <v>14.964692395178746</v>
+        <v>9.064916118206348</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>30.0</v>
+        <v>33.0</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C19" t="n">
-        <v>3812.2520339599805</v>
+        <v>9423.24961501254</v>
       </c>
       <c r="D19" t="n">
-        <v>954979.2255851598</v>
+        <v>788301.5634397555</v>
       </c>
       <c r="E19" t="n">
-        <v>3.991973785214058</v>
+        <v>11.953863917120971</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>31.0</v>
+        <v>34.0</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C20" t="n">
-        <v>22967.942794251376</v>
+        <v>51471.692726499445</v>
       </c>
       <c r="D20" t="n">
-        <v>2409104.157907932</v>
+        <v>5274309.777003881</v>
       </c>
       <c r="E20" t="n">
-        <v>9.533810615393547</v>
+        <v>9.758943805484705</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>33.0</v>
+        <v>35.0</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" t="n">
-        <v>12456.047162647177</v>
+        <v>8857.142946737338</v>
       </c>
       <c r="D21" t="n">
-        <v>1051183.584662591</v>
+        <v>1327496.3453727677</v>
       </c>
       <c r="E21" t="n">
-        <v>11.84954497424474</v>
+        <v>6.6720657858008705</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>34.0</v>
+        <v>36.0</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C22" t="n">
-        <v>51471.692726499445</v>
+        <v>221226.36562273267</v>
       </c>
       <c r="D22" t="n">
-        <v>5274309.777003881</v>
+        <v>1.5027480545143578E7</v>
       </c>
       <c r="E22" t="n">
-        <v>9.758943805484705</v>
+        <v>14.721454135851552</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>35.0</v>
+        <v>39.0</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" t="n">
-        <v>8857.142946737338</v>
+        <v>71567.97481901593</v>
       </c>
       <c r="D23" t="n">
-        <v>1327496.3453727677</v>
+        <v>4755244.714276284</v>
       </c>
       <c r="E23" t="n">
-        <v>6.6720657858008705</v>
+        <v>15.050324246016872</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C24" t="n">
-        <v>270637.3256250884</v>
+        <v>24627.721388718226</v>
       </c>
       <c r="D24" t="n">
-        <v>1.8869984035205126E7</v>
+        <v>2285659.3166476926</v>
       </c>
       <c r="E24" t="n">
-        <v>14.342212750162853</v>
+        <v>10.774887232467767</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>39.0</v>
+        <v>41.0</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C25" t="n">
-        <v>71567.97481901593</v>
+        <v>8328.024176806282</v>
       </c>
       <c r="D25" t="n">
-        <v>4755244.714276284</v>
+        <v>752767.6262806169</v>
       </c>
       <c r="E25" t="n">
-        <v>15.050324246016872</v>
+        <v>11.063207138641959</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>40.0</v>
+        <v>42.0</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C26" t="n">
-        <v>24627.721388718226</v>
+        <v>62291.57800717453</v>
       </c>
       <c r="D26" t="n">
-        <v>2285659.3166476926</v>
+        <v>4733924.715291146</v>
       </c>
       <c r="E26" t="n">
-        <v>10.774887232467767</v>
+        <v>13.158548509646815</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>41.0</v>
+        <v>44.0</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C27" t="n">
-        <v>8328.024176806282</v>
+        <v>5476.426426490039</v>
       </c>
       <c r="D27" t="n">
-        <v>752767.6262806169</v>
+        <v>384116.9213563548</v>
       </c>
       <c r="E27" t="n">
-        <v>11.063207138641959</v>
+        <v>14.257186085820528</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>42.0</v>
+        <v>48.0</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C28" t="n">
-        <v>62291.57800717453</v>
+        <v>381999.04549088026</v>
       </c>
       <c r="D28" t="n">
-        <v>4733924.715291146</v>
+        <v>2.299202296837785E7</v>
       </c>
       <c r="E28" t="n">
-        <v>13.158548509646815</v>
+        <v>16.61441648767765</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>44.0</v>
+        <v>49.0</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C29" t="n">
-        <v>5476.426426490039</v>
+        <v>30221.406332381404</v>
       </c>
       <c r="D29" t="n">
-        <v>384116.9213563548</v>
+        <v>2902955.358223645</v>
       </c>
       <c r="E29" t="n">
-        <v>14.257186085820528</v>
+        <v>10.410565304343592</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>48.0</v>
+        <v>50.0</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C30" t="n">
-        <v>461447.07912243827</v>
+        <v>6498.410650110485</v>
       </c>
       <c r="D30" t="n">
-        <v>2.8510542788351804E7</v>
+        <v>563279.5559912089</v>
       </c>
       <c r="E30" t="n">
-        <v>16.18513833805247</v>
+        <v>11.536741536225586</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>49.0</v>
+        <v>53.0</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C31" t="n">
-        <v>30221.406332381404</v>
+        <v>18647.25128699706</v>
       </c>
       <c r="D31" t="n">
-        <v>2902955.358223645</v>
+        <v>2752372.813938709</v>
       </c>
       <c r="E31" t="n">
-        <v>10.410565304343592</v>
+        <v>6.774972922477175</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>50.0</v>
+        <v>54.0</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C32" t="n">
-        <v>8075.862190644024</v>
+        <v>3846.644645155366</v>
       </c>
       <c r="D32" t="n">
-        <v>680228.8003994031</v>
+        <v>325031.2108367552</v>
       </c>
       <c r="E32" t="n">
-        <v>11.872273249680404</v>
+        <v>11.834693152244132</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>53.0</v>
+        <v>55.0</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C33" t="n">
-        <v>18647.25128699706</v>
+        <v>14403.531708608236</v>
       </c>
       <c r="D33" t="n">
-        <v>2752372.813938709</v>
+        <v>1174446.719861135</v>
       </c>
       <c r="E33" t="n">
-        <v>6.774972922477175</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="B34" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" t="n">
-        <v>3846.644645155366</v>
-      </c>
-      <c r="D34" t="n">
-        <v>325031.2108367552</v>
-      </c>
-      <c r="E34" t="n">
-        <v>11.834693152244132</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="B35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" t="n">
-        <v>28807.063417216472</v>
-      </c>
-      <c r="D35" t="n">
-        <v>2348893.43972227</v>
-      </c>
-      <c r="E35" t="n">
         <v>12.264099737373606</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wrote bullit points for asthma IR data analysis
</commit_message>
<xml_diff>
--- a/Results/Asthma_IR.xlsx
+++ b/Results/Asthma_IR.xlsx
@@ -11,13 +11,12 @@
     <sheet name="2008" r:id="rId5" sheetId="3"/>
     <sheet name="2009" r:id="rId6" sheetId="4"/>
     <sheet name="2010" r:id="rId7" sheetId="5"/>
-    <sheet name="Aggregate" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="56">
   <si>
     <t>FIPS</t>
   </si>
@@ -185,9 +184,6 @@
   </si>
   <si>
     <t>Wyoming</t>
-  </si>
-  <si>
-    <t>IR per 1000</t>
   </si>
 </sst>
 </file>
@@ -3791,578 +3787,4 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="n">
-        <v>42621.918836024626</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2802421.7470672023</v>
-      </c>
-      <c r="E2" t="n">
-        <v>15.208959493919652</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="n">
-        <v>156599.0264181489</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.6850453394726697E7</v>
-      </c>
-      <c r="E3" t="n">
-        <v>9.29346070101331</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>32938.5229378051</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2734477.7688722718</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12.045635664973537</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3184.446344618885</v>
-      </c>
-      <c r="D5" t="n">
-        <v>179492.85599165817</v>
-      </c>
-      <c r="E5" t="n">
-        <v>17.74135425627681</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="n">
-        <v>94786.03809289802</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.0458073543508092E7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>9.063431969431596</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="n">
-        <v>37799.24289699028</v>
-      </c>
-      <c r="D7" t="n">
-        <v>5673571.265652148</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6.662336846956915</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="n">
-        <v>105218.93189138013</v>
-      </c>
-      <c r="D8" t="n">
-        <v>6936762.371679282</v>
-      </c>
-      <c r="E8" t="n">
-        <v>15.168305652354107</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="n">
-        <v>11510.486502884885</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1829733.9661702944</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6.290797851327419</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="n">
-        <v>27509.487892604753</v>
-      </c>
-      <c r="D10" t="n">
-        <v>3059760.3617240055</v>
-      </c>
-      <c r="E10" t="n">
-        <v>8.990732815789757</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="n">
-        <v>5378.786540781787</v>
-      </c>
-      <c r="D11" t="n">
-        <v>931966.3594570106</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5.771438514063552</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>23.0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="n">
-        <v>6662.149701015229</v>
-      </c>
-      <c r="D12" t="n">
-        <v>722763.1937653258</v>
-      </c>
-      <c r="E12" t="n">
-        <v>9.217610634415294</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="n">
-        <v>64870.5736086545</v>
-      </c>
-      <c r="D13" t="n">
-        <v>5816583.904105316</v>
-      </c>
-      <c r="E13" t="n">
-        <v>11.152692831073782</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="n">
-        <v>126101.97053771566</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.0491065363787048E7</v>
-      </c>
-      <c r="E14" t="n">
-        <v>12.0199394594369</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>28.0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="n">
-        <v>18264.008952066375</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1300916.7417331804</v>
-      </c>
-      <c r="E15" t="n">
-        <v>14.039337312035567</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>29.0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="n">
-        <v>46410.034572168624</v>
-      </c>
-      <c r="D16" t="n">
-        <v>3600272.063188931</v>
-      </c>
-      <c r="E16" t="n">
-        <v>12.890702079625912</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>30.0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" t="n">
-        <v>3295.889765187216</v>
-      </c>
-      <c r="D17" t="n">
-        <v>768012.0066596719</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4.291456040540417</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>31.0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="n">
-        <v>18262.226573581298</v>
-      </c>
-      <c r="D18" t="n">
-        <v>2014605.1364890952</v>
-      </c>
-      <c r="E18" t="n">
-        <v>9.064916118206348</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="n">
-        <v>9423.24961501254</v>
-      </c>
-      <c r="D19" t="n">
-        <v>788301.5634397555</v>
-      </c>
-      <c r="E19" t="n">
-        <v>11.953863917120971</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>34.0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="n">
-        <v>51471.692726499445</v>
-      </c>
-      <c r="D20" t="n">
-        <v>5274309.777003881</v>
-      </c>
-      <c r="E20" t="n">
-        <v>9.758943805484705</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" t="n">
-        <v>8857.142946737338</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1327496.3453727677</v>
-      </c>
-      <c r="E21" t="n">
-        <v>6.6720657858008705</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" t="n">
-        <v>221226.36562273267</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1.5027480545143578E7</v>
-      </c>
-      <c r="E22" t="n">
-        <v>14.721454135851552</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="n">
-        <v>71567.97481901593</v>
-      </c>
-      <c r="D23" t="n">
-        <v>4755244.714276284</v>
-      </c>
-      <c r="E23" t="n">
-        <v>15.050324246016872</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>40.0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="n">
-        <v>24627.721388718226</v>
-      </c>
-      <c r="D24" t="n">
-        <v>2285659.3166476926</v>
-      </c>
-      <c r="E24" t="n">
-        <v>10.774887232467767</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>41.0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="n">
-        <v>8328.024176806282</v>
-      </c>
-      <c r="D25" t="n">
-        <v>752767.6262806169</v>
-      </c>
-      <c r="E25" t="n">
-        <v>11.063207138641959</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>42.0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" t="n">
-        <v>62291.57800717453</v>
-      </c>
-      <c r="D26" t="n">
-        <v>4733924.715291146</v>
-      </c>
-      <c r="E26" t="n">
-        <v>13.158548509646815</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" t="n">
-        <v>5476.426426490039</v>
-      </c>
-      <c r="D27" t="n">
-        <v>384116.9213563548</v>
-      </c>
-      <c r="E27" t="n">
-        <v>14.257186085820528</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="n">
-        <v>381999.04549088026</v>
-      </c>
-      <c r="D28" t="n">
-        <v>2.299202296837785E7</v>
-      </c>
-      <c r="E28" t="n">
-        <v>16.61441648767765</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>49.0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" t="n">
-        <v>30221.406332381404</v>
-      </c>
-      <c r="D29" t="n">
-        <v>2902955.358223645</v>
-      </c>
-      <c r="E29" t="n">
-        <v>10.410565304343592</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="n">
-        <v>6498.410650110485</v>
-      </c>
-      <c r="D30" t="n">
-        <v>563279.5559912089</v>
-      </c>
-      <c r="E30" t="n">
-        <v>11.536741536225586</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" t="n">
-        <v>18647.25128699706</v>
-      </c>
-      <c r="D31" t="n">
-        <v>2752372.813938709</v>
-      </c>
-      <c r="E31" t="n">
-        <v>6.774972922477175</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" t="n">
-        <v>3846.644645155366</v>
-      </c>
-      <c r="D32" t="n">
-        <v>325031.2108367552</v>
-      </c>
-      <c r="E32" t="n">
-        <v>11.834693152244132</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="B33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" t="n">
-        <v>14403.531708608236</v>
-      </c>
-      <c r="D33" t="n">
-        <v>1174446.719861135</v>
-      </c>
-      <c r="E33" t="n">
-        <v>12.264099737373606</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added the count data table for national and by state, added Asthma_IR_4 script, adjusted the plots, worked on the methods section
</commit_message>
<xml_diff>
--- a/Results/Asthma_IR.xlsx
+++ b/Results/Asthma_IR.xlsx
@@ -11,12 +11,13 @@
     <sheet name="2008" r:id="rId5" sheetId="3"/>
     <sheet name="2009" r:id="rId6" sheetId="4"/>
     <sheet name="2010" r:id="rId7" sheetId="5"/>
+    <sheet name="Aggregate" r:id="rId8" sheetId="6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="57">
   <si>
     <t>FIPS</t>
   </si>
@@ -184,6 +185,9 @@
   </si>
   <si>
     <t>Wyoming</t>
+  </si>
+  <si>
+    <t>IR per 1000</t>
   </si>
 </sst>
 </file>
@@ -3787,4 +3791,578 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>42621.918836024626</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2802421.7470672023</v>
+      </c>
+      <c r="E2" t="n">
+        <v>15.208959493919652</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="n">
+        <v>156599.0264181489</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.6850453394726697E7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9.29346070101331</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="n">
+        <v>32938.5229378051</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2734477.7688722718</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12.045635664973537</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3184.446344618885</v>
+      </c>
+      <c r="D5" t="n">
+        <v>179492.85599165817</v>
+      </c>
+      <c r="E5" t="n">
+        <v>17.74135425627681</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>94786.03809289802</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.0458073543508092E7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>9.063431969431596</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n">
+        <v>37799.24289699028</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5673571.265652148</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6.662336846956915</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="n">
+        <v>105218.93189138013</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6936762.371679282</v>
+      </c>
+      <c r="E8" t="n">
+        <v>15.168305652354107</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="n">
+        <v>11510.486502884885</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1829733.9661702944</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6.290797851327419</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>27509.487892604753</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3059760.3617240055</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8.990732815789757</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5378.786540781787</v>
+      </c>
+      <c r="D11" t="n">
+        <v>931966.3594570106</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5.771438514063552</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6662.149701015229</v>
+      </c>
+      <c r="D12" t="n">
+        <v>722763.1937653258</v>
+      </c>
+      <c r="E12" t="n">
+        <v>9.217610634415294</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="n">
+        <v>64870.5736086545</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5816583.904105316</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11.152692831073782</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="n">
+        <v>126101.97053771566</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.0491065363787048E7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12.0199394594369</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="n">
+        <v>18264.008952066375</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1300916.7417331804</v>
+      </c>
+      <c r="E15" t="n">
+        <v>14.039337312035567</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="n">
+        <v>46410.034572168624</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3600272.063188931</v>
+      </c>
+      <c r="E16" t="n">
+        <v>12.890702079625912</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3295.889765187216</v>
+      </c>
+      <c r="D17" t="n">
+        <v>768012.0066596719</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4.291456040540417</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="n">
+        <v>18262.226573581298</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2014605.1364890952</v>
+      </c>
+      <c r="E18" t="n">
+        <v>9.064916118206348</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9423.24961501254</v>
+      </c>
+      <c r="D19" t="n">
+        <v>788301.5634397555</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11.953863917120971</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="n">
+        <v>51471.692726499445</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5274309.777003881</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.758943805484705</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8857.142946737338</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1327496.3453727677</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6.6720657858008705</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="n">
+        <v>221226.36562273267</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.5027480545143578E7</v>
+      </c>
+      <c r="E22" t="n">
+        <v>14.721454135851552</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="n">
+        <v>71567.97481901593</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4755244.714276284</v>
+      </c>
+      <c r="E23" t="n">
+        <v>15.050324246016872</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="n">
+        <v>24627.721388718226</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2285659.3166476926</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10.774887232467767</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="n">
+        <v>8328.024176806282</v>
+      </c>
+      <c r="D25" t="n">
+        <v>752767.6262806169</v>
+      </c>
+      <c r="E25" t="n">
+        <v>11.063207138641959</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="n">
+        <v>62291.57800717453</v>
+      </c>
+      <c r="D26" t="n">
+        <v>4733924.715291146</v>
+      </c>
+      <c r="E26" t="n">
+        <v>13.158548509646815</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" t="n">
+        <v>5476.426426490039</v>
+      </c>
+      <c r="D27" t="n">
+        <v>384116.9213563548</v>
+      </c>
+      <c r="E27" t="n">
+        <v>14.257186085820528</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" t="n">
+        <v>381999.04549088026</v>
+      </c>
+      <c r="D28" t="n">
+        <v>2.299202296837785E7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>16.61441648767765</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="n">
+        <v>30221.406332381404</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2902955.358223645</v>
+      </c>
+      <c r="E29" t="n">
+        <v>10.410565304343592</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="n">
+        <v>6498.410650110485</v>
+      </c>
+      <c r="D30" t="n">
+        <v>563279.5559912089</v>
+      </c>
+      <c r="E30" t="n">
+        <v>11.536741536225586</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="n">
+        <v>18647.25128699706</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2752372.813938709</v>
+      </c>
+      <c r="E31" t="n">
+        <v>6.774972922477175</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3846.644645155366</v>
+      </c>
+      <c r="D32" t="n">
+        <v>325031.2108367552</v>
+      </c>
+      <c r="E32" t="n">
+        <v>11.834693152244132</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" t="n">
+        <v>14403.531708608236</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1174446.719861135</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12.264099737373606</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>